<commit_message>
removed comments. Added restock keyword in domain excel. Added review transactions senentce in dataelements.
</commit_message>
<xml_diff>
--- a/SoftwareDesignUsingNLP/data/DataElements.xlsx
+++ b/SoftwareDesignUsingNLP/data/DataElements.xlsx
@@ -1,20 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\373954\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="19200" windowHeight="6570" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14955" windowHeight="4140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Banking-Dataelements" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -164,9 +160,6 @@
     <t>Cred_Score</t>
   </si>
   <si>
-    <t>Account number of the customer will be used to deposit,withdrawal, verififcation, and other banking activities</t>
-  </si>
-  <si>
     <t xml:space="preserve">Customer Name  and will be used for verification, deposit , withdrawal, transfer of money and for all activities </t>
   </si>
   <si>
@@ -177,6 +170,9 @@
   </si>
   <si>
     <t>For approving loan one has to perform credit check score which is obtained from external agencies</t>
+  </si>
+  <si>
+    <t>Account number of the customer will be used to deposit,withdrawal, verififcation, and other banking activities. It is used to review transactions</t>
   </si>
 </sst>
 </file>
@@ -621,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -651,10 +647,10 @@
         <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -662,7 +658,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -728,7 +724,7 @@
         <v>28</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -772,7 +768,7 @@
         <v>38</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -816,7 +812,7 @@
         <v>45</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>